<commit_message>
Wijzigingen en aanvullingen tijdreeksen.
</commit_message>
<xml_diff>
--- a/_book/data/advertenties.xlsx
+++ b/_book/data/advertenties.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\office\forecasting_excel\hulpbestanden\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2647E61-0007-48A8-B4E1-7B8874E33239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="prog001" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -29,17 +34,13 @@
     <t>week</t>
   </si>
   <si>
-    <t>inkomsten
-(x1000 €)</t>
+    <t>inkomsten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,7 +72,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -351,7 +352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -359,7 +360,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -375,7 +376,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -383,7 +384,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>2.4980000000000002</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -391,7 +392,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>3.6840000000000002</v>
+        <v>3684</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -399,7 +400,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>5.1619999999999999</v>
+        <v>5162</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -407,7 +408,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>6.6120000000000001</v>
+        <v>6612</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -415,7 +416,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>8.375</v>
+        <v>8375</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -423,7 +424,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1">
-        <v>9.4120000000000008</v>
+        <v>9412</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -431,7 +432,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>10.88</v>
+        <v>10880</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -439,7 +440,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1">
-        <v>11.798999999999999</v>
+        <v>11799</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -447,7 +448,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>13.211</v>
+        <v>13211</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -455,7 +456,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="1">
-        <v>14.14</v>
+        <v>14140</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -463,7 +464,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>16.652000000000001</v>
+        <v>16652</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -471,7 +472,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="1">
-        <v>18.709</v>
+        <v>18709</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -479,7 +480,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="1">
-        <v>19.449000000000002</v>
+        <v>19449</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -487,7 +488,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="1">
-        <v>18.398</v>
+        <v>18398</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -495,7 +496,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="1">
-        <v>17.312000000000001</v>
+        <v>17312</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -503,7 +504,7 @@
         <v>32</v>
       </c>
       <c r="B18" s="1">
-        <v>14.186</v>
+        <v>14186</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,10 +512,11 @@
         <v>34</v>
       </c>
       <c r="B19" s="1">
-        <v>7.0529999999999999</v>
+        <v>7053</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>